<commit_message>
* DAC buf disabled * Current setup and measure constants adjusted
</commit_message>
<xml_diff>
--- a/HandyDevices/BrainEnchanter/Расчеты.xlsx
+++ b/HandyDevices/BrainEnchanter/Расчеты.xlsx
@@ -23,9 +23,41 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>Current setup</t>
+  </si>
+  <si>
+    <t>Dac1</t>
+  </si>
+  <si>
+    <t>I1,uA</t>
+  </si>
+  <si>
+    <t>DAC2</t>
+  </si>
+  <si>
+    <t>I2,uA</t>
+  </si>
+  <si>
+    <t>Divider</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Ur100,mV</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +65,69 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -50,14 +135,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,12 +458,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f>B3*10</f>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>298.39999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <f>B6*10</f>
+        <v>2984</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
+        <f>B7-B4</f>
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <f>B5-B2</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B2*B8-B4*B9</f>
+        <v>-104000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>